<commit_message>
#59106 UPD: admin report fixes
</commit_message>
<xml_diff>
--- a/www/local/modules/kelnik.report/export_tmpl/tables.xlsx
+++ b/www/local/modules/kelnik.report/export_tmpl/tables.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\server\www\oez\www\local\modules\kelnik.report\export_tmpl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="180" windowWidth="15195" windowHeight="11700" activeTab="2"/>
+    <workbookView xWindow="6036" yWindow="180" windowWidth="15192" windowHeight="11700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ф-1(общая)" sheetId="7" r:id="rId1"/>
@@ -457,7 +452,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
   </numFmts>
@@ -1078,20 +1073,20 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1102,86 +1097,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1192,6 +1118,114 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1203,33 +1237,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1246,6 +1253,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1254,37 +1264,22 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1368,7 +1363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1403,7 +1398,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1622,52 +1617,52 @@
       <selection pane="bottomLeft" activeCell="D10" sqref="D10:V10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" customWidth="1"/>
-    <col min="21" max="21" width="12.5703125" customWidth="1"/>
-    <col min="22" max="22" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.109375" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" customWidth="1"/>
+    <col min="21" max="21" width="12.5546875" customWidth="1"/>
+    <col min="22" max="22" width="25.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="22"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="110"/>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="110"/>
-      <c r="R1" s="110"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
       <c r="S1" s="16"/>
       <c r="T1" s="16"/>
       <c r="U1" s="16"/>
@@ -1676,51 +1671,51 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="80" t="s">
+      <c r="E2" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
       <c r="S2" s="47"/>
     </row>
     <row r="3" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="117" t="s">
+      <c r="E3" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117"/>
-      <c r="L3" s="118" t="s">
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
     </row>
-    <row r="4" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="24"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1742,20 +1737,20 @@
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
     </row>
-    <row r="5" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="102" t="s">
+    <row r="5" spans="1:22" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="101" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="107" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="84" t="s">
@@ -1764,151 +1759,151 @@
       <c r="G5" s="85"/>
       <c r="H5" s="85"/>
       <c r="I5" s="86"/>
-      <c r="J5" s="81" t="s">
+      <c r="J5" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="111" t="s">
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="113"/>
-      <c r="R5" s="97" t="s">
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="89"/>
+      <c r="R5" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="114"/>
-      <c r="T5" s="97" t="s">
+      <c r="S5" s="91"/>
+      <c r="T5" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="U5" s="98"/>
-      <c r="V5" s="92" t="s">
+      <c r="U5" s="104"/>
+      <c r="V5" s="107" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="103"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="146"/>
+    <row r="6" spans="1:22" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="102"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="118"/>
       <c r="D6" s="99"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="95" t="s">
+      <c r="E6" s="115"/>
+      <c r="F6" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95" t="s">
+      <c r="G6" s="80"/>
+      <c r="H6" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="95"/>
-      <c r="J6" s="107" t="s">
+      <c r="I6" s="80"/>
+      <c r="J6" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="108"/>
-      <c r="L6" s="107" t="s">
+      <c r="K6" s="83"/>
+      <c r="L6" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="109"/>
-      <c r="N6" s="107" t="s">
+      <c r="M6" s="96"/>
+      <c r="N6" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="108"/>
-      <c r="P6" s="107" t="s">
+      <c r="O6" s="83"/>
+      <c r="P6" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="109"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="116"/>
+      <c r="Q6" s="96"/>
+      <c r="R6" s="92"/>
+      <c r="S6" s="93"/>
       <c r="T6" s="99"/>
-      <c r="U6" s="100"/>
-      <c r="V6" s="105"/>
-    </row>
-    <row r="7" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="103"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="146"/>
+      <c r="U6" s="105"/>
+      <c r="V6" s="108"/>
+    </row>
+    <row r="7" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="102"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="118"/>
       <c r="D7" s="99"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="95" t="s">
+      <c r="E7" s="115"/>
+      <c r="F7" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="95" t="s">
+      <c r="G7" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="95" t="s">
+      <c r="H7" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="95" t="s">
+      <c r="J7" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="95" t="s">
+      <c r="K7" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="95" t="s">
+      <c r="L7" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="95" t="s">
+      <c r="M7" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="95" t="s">
+      <c r="N7" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="95" t="s">
+      <c r="O7" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="95" t="s">
+      <c r="P7" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="95" t="s">
+      <c r="Q7" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="R7" s="95" t="s">
+      <c r="R7" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="S7" s="95" t="s">
+      <c r="S7" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="T7" s="95" t="s">
+      <c r="T7" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="U7" s="95" t="s">
+      <c r="U7" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="105"/>
-    </row>
-    <row r="8" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="95"/>
-      <c r="I8" s="95"/>
-      <c r="J8" s="95"/>
-      <c r="K8" s="95"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="95"/>
-      <c r="N8" s="95"/>
-      <c r="O8" s="95"/>
-      <c r="P8" s="95"/>
-      <c r="Q8" s="95"/>
-      <c r="R8" s="95"/>
-      <c r="S8" s="95"/>
-      <c r="T8" s="95"/>
-      <c r="U8" s="95"/>
-      <c r="V8" s="106"/>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="V7" s="108"/>
+    </row>
+    <row r="8" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="103"/>
+      <c r="B8" s="114"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="80"/>
+      <c r="T8" s="80"/>
+      <c r="U8" s="80"/>
+      <c r="V8" s="109"/>
+    </row>
+    <row r="9" spans="1:22" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
         <v>1</v>
       </c>
-      <c r="B9" s="148">
+      <c r="B9" s="79">
         <v>2</v>
       </c>
       <c r="C9" s="17">
@@ -1972,7 +1967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="49">
         <v>1</v>
       </c>
@@ -1998,14 +1993,14 @@
       <c r="U10" s="26"/>
       <c r="V10" s="28"/>
     </row>
-    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="82" t="s">
+    <row r="11" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
       <c r="F11" s="52">
         <f t="shared" ref="F11:U11" si="0">SUM(F10:F10)</f>
         <v>0</v>
@@ -2072,7 +2067,7 @@
       </c>
       <c r="V11" s="52"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" s="31"/>
       <c r="C12" s="32"/>
@@ -2096,7 +2091,7 @@
       <c r="U12" s="33"/>
       <c r="V12" s="33"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
       <c r="B13" s="31"/>
       <c r="C13" s="32"/>
@@ -2120,83 +2115,83 @@
       <c r="U13" s="33"/>
       <c r="V13" s="33"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="83" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="83"/>
-      <c r="N14" s="83"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="83"/>
-      <c r="Q14" s="83"/>
-      <c r="R14" s="83"/>
-      <c r="S14" s="83"/>
-      <c r="T14" s="83"/>
-      <c r="U14" s="83"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="98"/>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98"/>
+      <c r="O14" s="98"/>
+      <c r="P14" s="98"/>
+      <c r="Q14" s="98"/>
+      <c r="R14" s="98"/>
+      <c r="S14" s="98"/>
+      <c r="T14" s="98"/>
+      <c r="U14" s="98"/>
       <c r="V14" s="51"/>
     </row>
-    <row r="15" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="83" t="s">
+    <row r="15" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="83"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="83"/>
-      <c r="P15" s="83"/>
-      <c r="Q15" s="83"/>
-      <c r="R15" s="83"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="83"/>
-      <c r="U15" s="83"/>
-      <c r="V15" s="83"/>
-    </row>
-    <row r="16" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="83"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="83"/>
-      <c r="N16" s="83"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="83"/>
-      <c r="R16" s="83"/>
-      <c r="S16" s="83"/>
-      <c r="T16" s="83"/>
-      <c r="U16" s="83"/>
-      <c r="V16" s="83"/>
-    </row>
-    <row r="17" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="98"/>
+      <c r="P15" s="98"/>
+      <c r="Q15" s="98"/>
+      <c r="R15" s="98"/>
+      <c r="S15" s="98"/>
+      <c r="T15" s="98"/>
+      <c r="U15" s="98"/>
+      <c r="V15" s="98"/>
+    </row>
+    <row r="16" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="98"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="98"/>
+      <c r="P16" s="98"/>
+      <c r="Q16" s="98"/>
+      <c r="R16" s="98"/>
+      <c r="S16" s="98"/>
+      <c r="T16" s="98"/>
+      <c r="U16" s="98"/>
+      <c r="V16" s="98"/>
+    </row>
+    <row r="17" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="63"/>
       <c r="C17" s="51"/>
       <c r="D17" s="51"/>
@@ -2219,57 +2214,57 @@
       <c r="U17" s="51"/>
       <c r="V17" s="51"/>
     </row>
-    <row r="18" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="83" t="s">
+    <row r="18" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="83"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
-      <c r="R18" s="83"/>
-      <c r="S18" s="83"/>
-      <c r="T18" s="83"/>
-      <c r="U18" s="83"/>
-      <c r="V18" s="83"/>
-    </row>
-    <row r="19" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="83"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="83"/>
-      <c r="K19" s="83"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="83"/>
-      <c r="O19" s="83"/>
-      <c r="P19" s="83"/>
-      <c r="Q19" s="83"/>
-      <c r="R19" s="83"/>
-      <c r="S19" s="83"/>
-      <c r="T19" s="83"/>
-      <c r="U19" s="83"/>
-      <c r="V19" s="83"/>
-    </row>
-    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="98"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="98"/>
+      <c r="P18" s="98"/>
+      <c r="Q18" s="98"/>
+      <c r="R18" s="98"/>
+      <c r="S18" s="98"/>
+      <c r="T18" s="98"/>
+      <c r="U18" s="98"/>
+      <c r="V18" s="98"/>
+    </row>
+    <row r="19" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="98"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="98"/>
+      <c r="P19" s="98"/>
+      <c r="Q19" s="98"/>
+      <c r="R19" s="98"/>
+      <c r="S19" s="98"/>
+      <c r="T19" s="98"/>
+      <c r="U19" s="98"/>
+      <c r="V19" s="98"/>
+    </row>
+    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
       <c r="B20" s="63"/>
       <c r="C20" s="51"/>
@@ -2293,45 +2288,45 @@
       <c r="U20" s="51"/>
       <c r="V20" s="51"/>
     </row>
-    <row r="21" spans="1:22" ht="6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="83"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="83"/>
-      <c r="P21" s="83"/>
-      <c r="Q21" s="83"/>
-      <c r="R21" s="83"/>
-      <c r="S21" s="83"/>
-      <c r="T21" s="83"/>
-      <c r="U21" s="83"/>
-      <c r="V21" s="83"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="96" t="s">
+    <row r="21" spans="1:22" ht="6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="98"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="98"/>
+      <c r="P21" s="98"/>
+      <c r="Q21" s="98"/>
+      <c r="R21" s="98"/>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="98"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="97"/>
+      <c r="I22" s="97"/>
+      <c r="J22" s="97"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
       <c r="M22" s="53"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
@@ -2343,35 +2338,65 @@
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="79" t="s">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="79" t="s">
+      <c r="B24" s="110"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="79" t="s">
+      <c r="B25" s="110"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="110"/>
+      <c r="E25" s="110"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="E2:R2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A14:U14"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="A15:V16"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A18:V19"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="A21:V21"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="T5:U6"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="V5:V8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="R7:R8"/>
     <mergeCell ref="U7:U8"/>
     <mergeCell ref="T7:T8"/>
     <mergeCell ref="E1:R1"/>
@@ -2388,36 +2413,6 @@
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="O7:O8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A18:V19"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="A21:V21"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="T5:U6"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="V5:V8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="E2:R2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A14:U14"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="A15:V16"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2439,75 +2434,75 @@
       <selection pane="bottomLeft" activeCell="E10" sqref="E10:AA10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
-    <col min="13" max="17" width="9.42578125" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" customWidth="1"/>
-    <col min="23" max="25" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" customWidth="1"/>
+    <col min="13" max="17" width="9.44140625" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" customWidth="1"/>
+    <col min="23" max="25" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="126" t="s">
+    <row r="1" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="W1" s="127" t="s">
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="W1" s="121" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="127"/>
-      <c r="Z1" s="127"/>
-      <c r="AA1" s="127"/>
+      <c r="X1" s="121"/>
+      <c r="Y1" s="121"/>
+      <c r="Z1" s="121"/>
+      <c r="AA1" s="121"/>
     </row>
     <row r="2" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
-      <c r="E2" s="119" t="s">
+      <c r="E2" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="119"/>
-      <c r="R2" s="119"/>
-      <c r="S2" s="119"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
+      <c r="M2" s="132"/>
+      <c r="N2" s="132"/>
+      <c r="O2" s="132"/>
+      <c r="P2" s="132"/>
+      <c r="Q2" s="132"/>
+      <c r="R2" s="132"/>
+      <c r="S2" s="132"/>
       <c r="T2" s="14"/>
       <c r="U2" s="14"/>
       <c r="V2" s="36"/>
@@ -2515,30 +2510,30 @@
       <c r="X2" s="36"/>
       <c r="Y2" s="36"/>
     </row>
-    <row r="3" spans="1:27" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>
-      <c r="F3" s="128" t="s">
+      <c r="F3" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="131" t="s">
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="131"/>
-      <c r="M3" s="131"/>
-      <c r="N3" s="131"/>
-      <c r="O3" s="131"/>
-      <c r="P3" s="131"/>
-      <c r="Q3" s="131"/>
-      <c r="R3" s="131"/>
-      <c r="S3" s="131"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="129"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="129"/>
+      <c r="Q3" s="129"/>
+      <c r="R3" s="129"/>
+      <c r="S3" s="129"/>
       <c r="T3" s="37"/>
       <c r="U3" s="37"/>
       <c r="V3" s="37"/>
@@ -2546,7 +2541,7 @@
       <c r="X3" s="37"/>
       <c r="Y3" s="37"/>
     </row>
-    <row r="4" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="37"/>
       <c r="C4" s="37"/>
@@ -2573,40 +2568,40 @@
       <c r="X4" s="37"/>
       <c r="Y4" s="37"/>
     </row>
-    <row r="5" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="81" t="s">
+    <row r="5" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="92" t="s">
+      <c r="C5" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="123"/>
-      <c r="I5" s="123"/>
-      <c r="J5" s="123"/>
-      <c r="K5" s="123"/>
-      <c r="L5" s="123"/>
-      <c r="M5" s="123"/>
-      <c r="N5" s="123"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="97" t="s">
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="123"/>
-      <c r="R5" s="123"/>
-      <c r="S5" s="123"/>
-      <c r="T5" s="123"/>
-      <c r="U5" s="123"/>
-      <c r="V5" s="123"/>
-      <c r="W5" s="98"/>
+      <c r="Q5" s="124"/>
+      <c r="R5" s="124"/>
+      <c r="S5" s="124"/>
+      <c r="T5" s="124"/>
+      <c r="U5" s="124"/>
+      <c r="V5" s="124"/>
+      <c r="W5" s="104"/>
       <c r="X5" s="84" t="s">
         <v>37</v>
       </c>
@@ -2616,90 +2611,90 @@
       </c>
       <c r="AA5" s="86"/>
     </row>
-    <row r="6" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="81"/>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="81" t="s">
+    <row r="6" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="106"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="125"/>
-      <c r="F6" s="89" t="s">
+      <c r="E6" s="131"/>
+      <c r="F6" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="91"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
+      <c r="M6" s="125"/>
+      <c r="N6" s="125"/>
+      <c r="O6" s="126"/>
       <c r="P6" s="99"/>
-      <c r="Q6" s="124"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="124"/>
-      <c r="T6" s="124"/>
-      <c r="U6" s="124"/>
-      <c r="V6" s="124"/>
-      <c r="W6" s="100"/>
-      <c r="X6" s="87"/>
-      <c r="Y6" s="88"/>
-      <c r="Z6" s="87"/>
-      <c r="AA6" s="88"/>
-    </row>
-    <row r="7" spans="1:27" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="81"/>
-      <c r="B7" s="93"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="95" t="s">
+      <c r="Q6" s="130"/>
+      <c r="R6" s="130"/>
+      <c r="S6" s="130"/>
+      <c r="T6" s="130"/>
+      <c r="U6" s="130"/>
+      <c r="V6" s="130"/>
+      <c r="W6" s="105"/>
+      <c r="X6" s="113"/>
+      <c r="Y6" s="123"/>
+      <c r="Z6" s="113"/>
+      <c r="AA6" s="123"/>
+    </row>
+    <row r="7" spans="1:27" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="106"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95" t="s">
+      <c r="G7" s="80"/>
+      <c r="H7" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95" t="s">
+      <c r="I7" s="80"/>
+      <c r="J7" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95" t="s">
+      <c r="K7" s="80"/>
+      <c r="L7" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="95"/>
-      <c r="N7" s="107" t="s">
+      <c r="M7" s="80"/>
+      <c r="N7" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="O7" s="108"/>
-      <c r="P7" s="97" t="s">
+      <c r="O7" s="83"/>
+      <c r="P7" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="129" t="s">
+      <c r="Q7" s="104"/>
+      <c r="R7" s="127" t="s">
         <v>46</v>
       </c>
-      <c r="S7" s="130"/>
-      <c r="T7" s="129" t="s">
+      <c r="S7" s="128"/>
+      <c r="T7" s="127" t="s">
         <v>47</v>
       </c>
-      <c r="U7" s="130"/>
-      <c r="V7" s="111" t="s">
+      <c r="U7" s="128"/>
+      <c r="V7" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="W7" s="113"/>
-      <c r="X7" s="89"/>
-      <c r="Y7" s="91"/>
-      <c r="Z7" s="87"/>
-      <c r="AA7" s="88"/>
-    </row>
-    <row r="8" spans="1:27" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="81"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
+      <c r="W7" s="89"/>
+      <c r="X7" s="114"/>
+      <c r="Y7" s="126"/>
+      <c r="Z7" s="113"/>
+      <c r="AA7" s="123"/>
+    </row>
+    <row r="8" spans="1:27" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="106"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
       <c r="D8" s="52" t="s">
         <v>49</v>
       </c>
@@ -2773,7 +2768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="65">
         <v>1</v>
       </c>
@@ -2856,7 +2851,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="65">
         <v>1</v>
       </c>
@@ -2887,12 +2882,12 @@
       <c r="Z10" s="39"/>
       <c r="AA10" s="39"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" s="120" t="s">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="121"/>
-      <c r="C11" s="122"/>
+      <c r="B11" s="134"/>
+      <c r="C11" s="135"/>
       <c r="D11" s="39">
         <f t="shared" ref="D11:AA11" si="0">SUM(D10:D10)</f>
         <v>0</v>
@@ -2990,80 +2985,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="83" t="s">
+    <row r="12" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="98" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="83"/>
-      <c r="R12" s="83"/>
-      <c r="S12" s="83"/>
-      <c r="T12" s="83"/>
-      <c r="U12" s="83"/>
-      <c r="V12" s="83"/>
-      <c r="W12" s="83"/>
-      <c r="X12" s="83"/>
-      <c r="Y12" s="83"/>
-      <c r="Z12" s="83"/>
-      <c r="AA12" s="83"/>
-    </row>
-    <row r="13" spans="1:27" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="83"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="83"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="83"/>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="83"/>
-      <c r="R13" s="83"/>
-      <c r="S13" s="83"/>
-      <c r="T13" s="83"/>
-      <c r="U13" s="83"/>
-      <c r="V13" s="83"/>
-      <c r="W13" s="83"/>
-      <c r="X13" s="83"/>
-      <c r="Y13" s="83"/>
-      <c r="Z13" s="83"/>
-      <c r="AA13" s="83"/>
-    </row>
-    <row r="14" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="83" t="s">
+      <c r="B12" s="98"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="98"/>
+      <c r="R12" s="98"/>
+      <c r="S12" s="98"/>
+      <c r="T12" s="98"/>
+      <c r="U12" s="98"/>
+      <c r="V12" s="98"/>
+      <c r="W12" s="98"/>
+      <c r="X12" s="98"/>
+      <c r="Y12" s="98"/>
+      <c r="Z12" s="98"/>
+      <c r="AA12" s="98"/>
+    </row>
+    <row r="13" spans="1:27" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="98"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="98"/>
+      <c r="Q13" s="98"/>
+      <c r="R13" s="98"/>
+      <c r="S13" s="98"/>
+      <c r="T13" s="98"/>
+      <c r="U13" s="98"/>
+      <c r="V13" s="98"/>
+      <c r="W13" s="98"/>
+      <c r="X13" s="98"/>
+      <c r="Y13" s="98"/>
+      <c r="Z13" s="98"/>
+      <c r="AA13" s="98"/>
+    </row>
+    <row r="14" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
       <c r="L14" s="51"/>
       <c r="M14" s="51"/>
       <c r="N14" s="51"/>
@@ -3081,126 +3076,138 @@
       <c r="Z14" s="51"/>
       <c r="AA14" s="51"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A16" s="83" t="s">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="83"/>
-      <c r="N16" s="83"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="83"/>
-      <c r="Q16" s="83"/>
-      <c r="R16" s="83"/>
-      <c r="S16" s="83"/>
-      <c r="T16" s="83"/>
-      <c r="U16" s="83"/>
-      <c r="V16" s="83"/>
-      <c r="W16" s="83"/>
-      <c r="X16" s="83"/>
-      <c r="Y16" s="83"/>
-      <c r="Z16" s="83"/>
-      <c r="AA16" s="83"/>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A17" s="83"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="83"/>
-      <c r="N17" s="83"/>
-      <c r="O17" s="83"/>
-      <c r="P17" s="83"/>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="83"/>
-      <c r="S17" s="83"/>
-      <c r="T17" s="83"/>
-      <c r="U17" s="83"/>
-      <c r="V17" s="83"/>
-      <c r="W17" s="83"/>
-      <c r="X17" s="83"/>
-      <c r="Y17" s="83"/>
-      <c r="Z17" s="83"/>
-      <c r="AA17" s="83"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="83"/>
-      <c r="O20" s="83"/>
-      <c r="P20" s="83"/>
-      <c r="Q20" s="83"/>
-      <c r="R20" s="83"/>
-      <c r="S20" s="83"/>
-      <c r="T20" s="83"/>
-      <c r="U20" s="83"/>
-      <c r="V20" s="83"/>
-      <c r="W20" s="83"/>
-      <c r="X20" s="83"/>
-      <c r="Y20" s="83"/>
-      <c r="Z20" s="83"/>
-      <c r="AA20" s="83"/>
-      <c r="AB20" s="83"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B21" s="83"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="83"/>
-      <c r="P21" s="83"/>
-      <c r="Q21" s="83"/>
-      <c r="R21" s="83"/>
-      <c r="S21" s="83"/>
-      <c r="T21" s="83"/>
-      <c r="U21" s="83"/>
-      <c r="V21" s="83"/>
-      <c r="W21" s="83"/>
-      <c r="X21" s="83"/>
-      <c r="Y21" s="83"/>
-      <c r="Z21" s="83"/>
-      <c r="AA21" s="83"/>
-      <c r="AB21" s="83"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="98"/>
+      <c r="P16" s="98"/>
+      <c r="Q16" s="98"/>
+      <c r="R16" s="98"/>
+      <c r="S16" s="98"/>
+      <c r="T16" s="98"/>
+      <c r="U16" s="98"/>
+      <c r="V16" s="98"/>
+      <c r="W16" s="98"/>
+      <c r="X16" s="98"/>
+      <c r="Y16" s="98"/>
+      <c r="Z16" s="98"/>
+      <c r="AA16" s="98"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="98"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="98"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="98"/>
+      <c r="M17" s="98"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="98"/>
+      <c r="P17" s="98"/>
+      <c r="Q17" s="98"/>
+      <c r="R17" s="98"/>
+      <c r="S17" s="98"/>
+      <c r="T17" s="98"/>
+      <c r="U17" s="98"/>
+      <c r="V17" s="98"/>
+      <c r="W17" s="98"/>
+      <c r="X17" s="98"/>
+      <c r="Y17" s="98"/>
+      <c r="Z17" s="98"/>
+      <c r="AA17" s="98"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B20" s="98"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="98"/>
+      <c r="I20" s="98"/>
+      <c r="J20" s="98"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="98"/>
+      <c r="O20" s="98"/>
+      <c r="P20" s="98"/>
+      <c r="Q20" s="98"/>
+      <c r="R20" s="98"/>
+      <c r="S20" s="98"/>
+      <c r="T20" s="98"/>
+      <c r="U20" s="98"/>
+      <c r="V20" s="98"/>
+      <c r="W20" s="98"/>
+      <c r="X20" s="98"/>
+      <c r="Y20" s="98"/>
+      <c r="Z20" s="98"/>
+      <c r="AA20" s="98"/>
+      <c r="AB20" s="98"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B21" s="98"/>
+      <c r="C21" s="98"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="98"/>
+      <c r="P21" s="98"/>
+      <c r="Q21" s="98"/>
+      <c r="R21" s="98"/>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="98"/>
+      <c r="W21" s="98"/>
+      <c r="X21" s="98"/>
+      <c r="Y21" s="98"/>
+      <c r="Z21" s="98"/>
+      <c r="AA21" s="98"/>
+      <c r="AB21" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="E2:S2"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="P5:W6"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="F1:S1"/>
     <mergeCell ref="W1:AA1"/>
     <mergeCell ref="B20:AB21"/>
@@ -3217,18 +3224,6 @@
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="P5:W6"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="E2:S2"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="V7:W7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3245,26 +3240,26 @@
   <dimension ref="A1:HU16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" customWidth="1"/>
+    <col min="8" max="9" width="30.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:229" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:229" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J1" s="58" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:229" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:229" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -3278,96 +3273,96 @@
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:229" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-    </row>
-    <row r="4" spans="1:229" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+    </row>
+    <row r="4" spans="1:229" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="47"/>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="118" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="118"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
     </row>
-    <row r="5" spans="1:229" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="138"/>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="138"/>
-      <c r="H5" s="138"/>
-      <c r="I5" s="138"/>
-      <c r="J5" s="138"/>
-    </row>
-    <row r="6" spans="1:229" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="133" t="s">
+    <row r="5" spans="1:229" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="140"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="140"/>
+      <c r="H5" s="140"/>
+      <c r="I5" s="140"/>
+      <c r="J5" s="140"/>
+    </row>
+    <row r="6" spans="1:229" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="133" t="s">
+      <c r="C6" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="133" t="s">
+      <c r="D6" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="136" t="s">
+      <c r="E6" s="141" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="137"/>
-      <c r="G6" s="133" t="s">
+      <c r="F6" s="142"/>
+      <c r="G6" s="137" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="135" t="s">
+      <c r="H6" s="139" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="133" t="s">
+      <c r="I6" s="137" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="135" t="s">
+      <c r="J6" s="139" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:229" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="134"/>
-      <c r="B7" s="135"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
+    <row r="7" spans="1:229" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="138"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
       <c r="E7" s="72" t="s">
         <v>62</v>
       </c>
       <c r="F7" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="134"/>
-      <c r="H7" s="135"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="135"/>
-    </row>
-    <row r="8" spans="1:229" x14ac:dyDescent="0.2">
+      <c r="G7" s="138"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="139"/>
+    </row>
+    <row r="8" spans="1:229" x14ac:dyDescent="0.25">
       <c r="A8" s="73">
         <v>1</v>
       </c>
@@ -3397,7 +3392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:229" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:229" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="74">
         <v>1</v>
       </c>
@@ -3411,270 +3406,291 @@
       <c r="I9" s="74"/>
       <c r="J9" s="74"/>
     </row>
-    <row r="11" spans="1:229" x14ac:dyDescent="0.2">
-      <c r="A11" s="132" t="s">
+    <row r="11" spans="1:229" x14ac:dyDescent="0.25">
+      <c r="A11" s="136" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="132"/>
-      <c r="C11" s="132"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132"/>
-      <c r="H11" s="132"/>
-      <c r="I11" s="132"/>
-      <c r="J11" s="132"/>
-    </row>
-    <row r="12" spans="1:229" x14ac:dyDescent="0.2">
-      <c r="A12" s="132"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="132"/>
-      <c r="H12" s="132"/>
-      <c r="I12" s="132"/>
-      <c r="J12" s="132"/>
-    </row>
-    <row r="16" spans="1:229" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="132" t="s">
+      <c r="B11" s="136"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="136"/>
+    </row>
+    <row r="12" spans="1:229" x14ac:dyDescent="0.25">
+      <c r="A12" s="136"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="136"/>
+      <c r="H12" s="136"/>
+      <c r="I12" s="136"/>
+      <c r="J12" s="136"/>
+    </row>
+    <row r="16" spans="1:229" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="136" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="132"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
-      <c r="I16" s="132"/>
-      <c r="J16" s="132"/>
-      <c r="K16" s="132"/>
-      <c r="L16" s="132"/>
-      <c r="M16" s="132"/>
-      <c r="N16" s="132"/>
-      <c r="O16" s="132"/>
-      <c r="P16" s="132"/>
-      <c r="Q16" s="132"/>
-      <c r="R16" s="132"/>
-      <c r="S16" s="132"/>
-      <c r="T16" s="132"/>
-      <c r="U16" s="132"/>
-      <c r="V16" s="132"/>
-      <c r="W16" s="132"/>
-      <c r="X16" s="132"/>
-      <c r="Y16" s="132"/>
-      <c r="Z16" s="132"/>
-      <c r="AA16" s="132"/>
-      <c r="AB16" s="132"/>
-      <c r="AC16" s="132"/>
-      <c r="AD16" s="132"/>
-      <c r="AE16" s="132"/>
-      <c r="AF16" s="132"/>
-      <c r="AG16" s="132"/>
-      <c r="AH16" s="132"/>
-      <c r="AI16" s="132"/>
-      <c r="AJ16" s="132"/>
-      <c r="AK16" s="132"/>
-      <c r="AL16" s="132"/>
-      <c r="AM16" s="132"/>
-      <c r="AN16" s="132"/>
-      <c r="AO16" s="132"/>
-      <c r="AP16" s="132"/>
-      <c r="AQ16" s="132"/>
-      <c r="AR16" s="132"/>
-      <c r="AS16" s="132"/>
-      <c r="AT16" s="132"/>
-      <c r="AU16" s="132"/>
-      <c r="AV16" s="132"/>
-      <c r="AW16" s="132"/>
-      <c r="AX16" s="132"/>
-      <c r="AY16" s="132"/>
-      <c r="AZ16" s="132"/>
-      <c r="BA16" s="132"/>
-      <c r="BB16" s="132"/>
-      <c r="BC16" s="132"/>
-      <c r="BD16" s="132"/>
-      <c r="BE16" s="132"/>
-      <c r="BF16" s="132"/>
-      <c r="BG16" s="132"/>
-      <c r="BH16" s="132"/>
-      <c r="BI16" s="132"/>
-      <c r="BJ16" s="132"/>
-      <c r="BK16" s="132"/>
-      <c r="BL16" s="132"/>
-      <c r="BM16" s="132"/>
-      <c r="BN16" s="132"/>
-      <c r="BO16" s="132"/>
-      <c r="BP16" s="132"/>
-      <c r="BQ16" s="132"/>
-      <c r="BR16" s="132"/>
-      <c r="BS16" s="132"/>
-      <c r="BT16" s="132"/>
-      <c r="BU16" s="132"/>
-      <c r="BV16" s="132"/>
-      <c r="BW16" s="132"/>
-      <c r="BX16" s="132"/>
-      <c r="BY16" s="132"/>
-      <c r="BZ16" s="132"/>
-      <c r="CA16" s="132"/>
-      <c r="CB16" s="132"/>
-      <c r="CC16" s="132"/>
-      <c r="CD16" s="132"/>
-      <c r="CE16" s="132"/>
-      <c r="CF16" s="132"/>
-      <c r="CG16" s="132"/>
-      <c r="CH16" s="132"/>
-      <c r="CI16" s="132"/>
-      <c r="CJ16" s="132"/>
-      <c r="CK16" s="132"/>
-      <c r="CL16" s="132"/>
-      <c r="CM16" s="132"/>
-      <c r="CN16" s="132"/>
-      <c r="CO16" s="132"/>
-      <c r="CP16" s="132"/>
-      <c r="CQ16" s="132"/>
-      <c r="CR16" s="132"/>
-      <c r="CS16" s="132"/>
-      <c r="CT16" s="132"/>
-      <c r="CU16" s="132"/>
-      <c r="CV16" s="132"/>
-      <c r="CW16" s="132"/>
-      <c r="CX16" s="132"/>
-      <c r="CY16" s="132"/>
-      <c r="CZ16" s="132"/>
-      <c r="DA16" s="132"/>
-      <c r="DB16" s="132"/>
-      <c r="DC16" s="132"/>
-      <c r="DD16" s="132"/>
-      <c r="DE16" s="132"/>
-      <c r="DF16" s="132"/>
-      <c r="DG16" s="132"/>
-      <c r="DH16" s="132"/>
-      <c r="DI16" s="132"/>
-      <c r="DJ16" s="132"/>
-      <c r="DK16" s="132"/>
-      <c r="DL16" s="132"/>
-      <c r="DM16" s="132"/>
-      <c r="DN16" s="132"/>
-      <c r="DO16" s="132"/>
-      <c r="DP16" s="132"/>
-      <c r="DQ16" s="132"/>
-      <c r="DR16" s="132"/>
-      <c r="DS16" s="132"/>
-      <c r="DT16" s="132"/>
-      <c r="DU16" s="132"/>
-      <c r="DV16" s="132"/>
-      <c r="DW16" s="132"/>
-      <c r="DX16" s="132"/>
-      <c r="DY16" s="132"/>
-      <c r="DZ16" s="132"/>
-      <c r="EA16" s="132"/>
-      <c r="EB16" s="132"/>
-      <c r="EC16" s="132"/>
-      <c r="ED16" s="132"/>
-      <c r="EE16" s="132"/>
-      <c r="EF16" s="132"/>
-      <c r="EG16" s="132"/>
-      <c r="EH16" s="132"/>
-      <c r="EI16" s="132"/>
-      <c r="EJ16" s="132"/>
-      <c r="EK16" s="132"/>
-      <c r="EL16" s="132"/>
-      <c r="EM16" s="132"/>
-      <c r="EN16" s="132"/>
-      <c r="EO16" s="132"/>
-      <c r="EP16" s="132"/>
-      <c r="EQ16" s="132"/>
-      <c r="ER16" s="132"/>
-      <c r="ES16" s="132"/>
-      <c r="ET16" s="132"/>
-      <c r="EU16" s="132"/>
-      <c r="EV16" s="132"/>
-      <c r="EW16" s="132"/>
-      <c r="EX16" s="132"/>
-      <c r="EY16" s="132"/>
-      <c r="EZ16" s="132"/>
-      <c r="FA16" s="132"/>
-      <c r="FB16" s="132"/>
-      <c r="FC16" s="132"/>
-      <c r="FD16" s="132"/>
-      <c r="FE16" s="132"/>
-      <c r="FF16" s="132"/>
-      <c r="FG16" s="132"/>
-      <c r="FH16" s="132"/>
-      <c r="FI16" s="132"/>
-      <c r="FJ16" s="132"/>
-      <c r="FK16" s="132"/>
-      <c r="FL16" s="132"/>
-      <c r="FM16" s="132"/>
-      <c r="FN16" s="132"/>
-      <c r="FO16" s="132"/>
-      <c r="FP16" s="132"/>
-      <c r="FQ16" s="132"/>
-      <c r="FR16" s="132"/>
-      <c r="FS16" s="132"/>
-      <c r="FT16" s="132"/>
-      <c r="FU16" s="132"/>
-      <c r="FV16" s="132"/>
-      <c r="FW16" s="132"/>
-      <c r="FX16" s="132"/>
-      <c r="FY16" s="132"/>
-      <c r="FZ16" s="132"/>
-      <c r="GA16" s="132"/>
-      <c r="GB16" s="132"/>
-      <c r="GC16" s="132"/>
-      <c r="GD16" s="132"/>
-      <c r="GE16" s="132"/>
-      <c r="GF16" s="132"/>
-      <c r="GG16" s="132"/>
-      <c r="GH16" s="132"/>
-      <c r="GI16" s="132"/>
-      <c r="GJ16" s="132"/>
-      <c r="GK16" s="132"/>
-      <c r="GL16" s="132"/>
-      <c r="GM16" s="132"/>
-      <c r="GN16" s="132"/>
-      <c r="GO16" s="132"/>
-      <c r="GP16" s="132"/>
-      <c r="GQ16" s="132"/>
-      <c r="GR16" s="132"/>
-      <c r="GS16" s="132"/>
-      <c r="GT16" s="132"/>
-      <c r="GU16" s="132"/>
-      <c r="GV16" s="132"/>
-      <c r="GW16" s="132"/>
-      <c r="GX16" s="132"/>
-      <c r="GY16" s="132"/>
-      <c r="GZ16" s="132"/>
-      <c r="HA16" s="132"/>
-      <c r="HB16" s="132"/>
-      <c r="HC16" s="132"/>
-      <c r="HD16" s="132"/>
-      <c r="HE16" s="132"/>
-      <c r="HF16" s="132"/>
-      <c r="HG16" s="132"/>
-      <c r="HH16" s="132"/>
-      <c r="HI16" s="132"/>
-      <c r="HJ16" s="132"/>
-      <c r="HK16" s="132"/>
-      <c r="HL16" s="132"/>
-      <c r="HM16" s="132"/>
-      <c r="HN16" s="132"/>
-      <c r="HO16" s="132"/>
-      <c r="HP16" s="132"/>
-      <c r="HQ16" s="132"/>
-      <c r="HR16" s="132"/>
-      <c r="HS16" s="132"/>
-      <c r="HT16" s="132"/>
-      <c r="HU16" s="132"/>
+      <c r="B16" s="136"/>
+      <c r="C16" s="136"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="136"/>
+      <c r="H16" s="136"/>
+      <c r="I16" s="136"/>
+      <c r="J16" s="136"/>
+      <c r="K16" s="136"/>
+      <c r="L16" s="136"/>
+      <c r="M16" s="136"/>
+      <c r="N16" s="136"/>
+      <c r="O16" s="136"/>
+      <c r="P16" s="136"/>
+      <c r="Q16" s="136"/>
+      <c r="R16" s="136"/>
+      <c r="S16" s="136"/>
+      <c r="T16" s="136"/>
+      <c r="U16" s="136"/>
+      <c r="V16" s="136"/>
+      <c r="W16" s="136"/>
+      <c r="X16" s="136"/>
+      <c r="Y16" s="136"/>
+      <c r="Z16" s="136"/>
+      <c r="AA16" s="136"/>
+      <c r="AB16" s="136"/>
+      <c r="AC16" s="136"/>
+      <c r="AD16" s="136"/>
+      <c r="AE16" s="136"/>
+      <c r="AF16" s="136"/>
+      <c r="AG16" s="136"/>
+      <c r="AH16" s="136"/>
+      <c r="AI16" s="136"/>
+      <c r="AJ16" s="136"/>
+      <c r="AK16" s="136"/>
+      <c r="AL16" s="136"/>
+      <c r="AM16" s="136"/>
+      <c r="AN16" s="136"/>
+      <c r="AO16" s="136"/>
+      <c r="AP16" s="136"/>
+      <c r="AQ16" s="136"/>
+      <c r="AR16" s="136"/>
+      <c r="AS16" s="136"/>
+      <c r="AT16" s="136"/>
+      <c r="AU16" s="136"/>
+      <c r="AV16" s="136"/>
+      <c r="AW16" s="136"/>
+      <c r="AX16" s="136"/>
+      <c r="AY16" s="136"/>
+      <c r="AZ16" s="136"/>
+      <c r="BA16" s="136"/>
+      <c r="BB16" s="136"/>
+      <c r="BC16" s="136"/>
+      <c r="BD16" s="136"/>
+      <c r="BE16" s="136"/>
+      <c r="BF16" s="136"/>
+      <c r="BG16" s="136"/>
+      <c r="BH16" s="136"/>
+      <c r="BI16" s="136"/>
+      <c r="BJ16" s="136"/>
+      <c r="BK16" s="136"/>
+      <c r="BL16" s="136"/>
+      <c r="BM16" s="136"/>
+      <c r="BN16" s="136"/>
+      <c r="BO16" s="136"/>
+      <c r="BP16" s="136"/>
+      <c r="BQ16" s="136"/>
+      <c r="BR16" s="136"/>
+      <c r="BS16" s="136"/>
+      <c r="BT16" s="136"/>
+      <c r="BU16" s="136"/>
+      <c r="BV16" s="136"/>
+      <c r="BW16" s="136"/>
+      <c r="BX16" s="136"/>
+      <c r="BY16" s="136"/>
+      <c r="BZ16" s="136"/>
+      <c r="CA16" s="136"/>
+      <c r="CB16" s="136"/>
+      <c r="CC16" s="136"/>
+      <c r="CD16" s="136"/>
+      <c r="CE16" s="136"/>
+      <c r="CF16" s="136"/>
+      <c r="CG16" s="136"/>
+      <c r="CH16" s="136"/>
+      <c r="CI16" s="136"/>
+      <c r="CJ16" s="136"/>
+      <c r="CK16" s="136"/>
+      <c r="CL16" s="136"/>
+      <c r="CM16" s="136"/>
+      <c r="CN16" s="136"/>
+      <c r="CO16" s="136"/>
+      <c r="CP16" s="136"/>
+      <c r="CQ16" s="136"/>
+      <c r="CR16" s="136"/>
+      <c r="CS16" s="136"/>
+      <c r="CT16" s="136"/>
+      <c r="CU16" s="136"/>
+      <c r="CV16" s="136"/>
+      <c r="CW16" s="136"/>
+      <c r="CX16" s="136"/>
+      <c r="CY16" s="136"/>
+      <c r="CZ16" s="136"/>
+      <c r="DA16" s="136"/>
+      <c r="DB16" s="136"/>
+      <c r="DC16" s="136"/>
+      <c r="DD16" s="136"/>
+      <c r="DE16" s="136"/>
+      <c r="DF16" s="136"/>
+      <c r="DG16" s="136"/>
+      <c r="DH16" s="136"/>
+      <c r="DI16" s="136"/>
+      <c r="DJ16" s="136"/>
+      <c r="DK16" s="136"/>
+      <c r="DL16" s="136"/>
+      <c r="DM16" s="136"/>
+      <c r="DN16" s="136"/>
+      <c r="DO16" s="136"/>
+      <c r="DP16" s="136"/>
+      <c r="DQ16" s="136"/>
+      <c r="DR16" s="136"/>
+      <c r="DS16" s="136"/>
+      <c r="DT16" s="136"/>
+      <c r="DU16" s="136"/>
+      <c r="DV16" s="136"/>
+      <c r="DW16" s="136"/>
+      <c r="DX16" s="136"/>
+      <c r="DY16" s="136"/>
+      <c r="DZ16" s="136"/>
+      <c r="EA16" s="136"/>
+      <c r="EB16" s="136"/>
+      <c r="EC16" s="136"/>
+      <c r="ED16" s="136"/>
+      <c r="EE16" s="136"/>
+      <c r="EF16" s="136"/>
+      <c r="EG16" s="136"/>
+      <c r="EH16" s="136"/>
+      <c r="EI16" s="136"/>
+      <c r="EJ16" s="136"/>
+      <c r="EK16" s="136"/>
+      <c r="EL16" s="136"/>
+      <c r="EM16" s="136"/>
+      <c r="EN16" s="136"/>
+      <c r="EO16" s="136"/>
+      <c r="EP16" s="136"/>
+      <c r="EQ16" s="136"/>
+      <c r="ER16" s="136"/>
+      <c r="ES16" s="136"/>
+      <c r="ET16" s="136"/>
+      <c r="EU16" s="136"/>
+      <c r="EV16" s="136"/>
+      <c r="EW16" s="136"/>
+      <c r="EX16" s="136"/>
+      <c r="EY16" s="136"/>
+      <c r="EZ16" s="136"/>
+      <c r="FA16" s="136"/>
+      <c r="FB16" s="136"/>
+      <c r="FC16" s="136"/>
+      <c r="FD16" s="136"/>
+      <c r="FE16" s="136"/>
+      <c r="FF16" s="136"/>
+      <c r="FG16" s="136"/>
+      <c r="FH16" s="136"/>
+      <c r="FI16" s="136"/>
+      <c r="FJ16" s="136"/>
+      <c r="FK16" s="136"/>
+      <c r="FL16" s="136"/>
+      <c r="FM16" s="136"/>
+      <c r="FN16" s="136"/>
+      <c r="FO16" s="136"/>
+      <c r="FP16" s="136"/>
+      <c r="FQ16" s="136"/>
+      <c r="FR16" s="136"/>
+      <c r="FS16" s="136"/>
+      <c r="FT16" s="136"/>
+      <c r="FU16" s="136"/>
+      <c r="FV16" s="136"/>
+      <c r="FW16" s="136"/>
+      <c r="FX16" s="136"/>
+      <c r="FY16" s="136"/>
+      <c r="FZ16" s="136"/>
+      <c r="GA16" s="136"/>
+      <c r="GB16" s="136"/>
+      <c r="GC16" s="136"/>
+      <c r="GD16" s="136"/>
+      <c r="GE16" s="136"/>
+      <c r="GF16" s="136"/>
+      <c r="GG16" s="136"/>
+      <c r="GH16" s="136"/>
+      <c r="GI16" s="136"/>
+      <c r="GJ16" s="136"/>
+      <c r="GK16" s="136"/>
+      <c r="GL16" s="136"/>
+      <c r="GM16" s="136"/>
+      <c r="GN16" s="136"/>
+      <c r="GO16" s="136"/>
+      <c r="GP16" s="136"/>
+      <c r="GQ16" s="136"/>
+      <c r="GR16" s="136"/>
+      <c r="GS16" s="136"/>
+      <c r="GT16" s="136"/>
+      <c r="GU16" s="136"/>
+      <c r="GV16" s="136"/>
+      <c r="GW16" s="136"/>
+      <c r="GX16" s="136"/>
+      <c r="GY16" s="136"/>
+      <c r="GZ16" s="136"/>
+      <c r="HA16" s="136"/>
+      <c r="HB16" s="136"/>
+      <c r="HC16" s="136"/>
+      <c r="HD16" s="136"/>
+      <c r="HE16" s="136"/>
+      <c r="HF16" s="136"/>
+      <c r="HG16" s="136"/>
+      <c r="HH16" s="136"/>
+      <c r="HI16" s="136"/>
+      <c r="HJ16" s="136"/>
+      <c r="HK16" s="136"/>
+      <c r="HL16" s="136"/>
+      <c r="HM16" s="136"/>
+      <c r="HN16" s="136"/>
+      <c r="HO16" s="136"/>
+      <c r="HP16" s="136"/>
+      <c r="HQ16" s="136"/>
+      <c r="HR16" s="136"/>
+      <c r="HS16" s="136"/>
+      <c r="HT16" s="136"/>
+      <c r="HU16" s="136"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:J9">
-    <filterColumn colId="4" showButton="0"/>
-  </autoFilter>
   <mergeCells count="40">
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="K16:S16"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A11:J12"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="DO16:DW16"/>
+    <mergeCell ref="DX16:EF16"/>
+    <mergeCell ref="EG16:EO16"/>
+    <mergeCell ref="EP16:EX16"/>
+    <mergeCell ref="AL16:AT16"/>
+    <mergeCell ref="AU16:BC16"/>
+    <mergeCell ref="BD16:BL16"/>
+    <mergeCell ref="BM16:BU16"/>
     <mergeCell ref="T16:AB16"/>
     <mergeCell ref="AC16:AK16"/>
     <mergeCell ref="HS16:HU16"/>
@@ -3691,30 +3707,6 @@
     <mergeCell ref="GR16:GZ16"/>
     <mergeCell ref="HA16:HI16"/>
     <mergeCell ref="HJ16:HR16"/>
-    <mergeCell ref="DO16:DW16"/>
-    <mergeCell ref="DX16:EF16"/>
-    <mergeCell ref="EG16:EO16"/>
-    <mergeCell ref="EP16:EX16"/>
-    <mergeCell ref="AL16:AT16"/>
-    <mergeCell ref="AU16:BC16"/>
-    <mergeCell ref="BD16:BL16"/>
-    <mergeCell ref="BM16:BU16"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="K16:S16"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A11:J12"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3737,28 +3729,28 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F1" s="58" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="110" t="s">
+    <row r="2" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B2" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14"/>
@@ -3769,56 +3761,56 @@
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="47"/>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="118" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="118"/>
+      <c r="F4" s="95"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="138"/>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="92" t="s">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="140"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
+      <c r="F5" s="140"/>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="80" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="94"/>
-      <c r="B7" s="95"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="116"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -3838,7 +3830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="65">
         <v>1</v>
       </c>
@@ -3848,47 +3840,47 @@
       <c r="E9" s="65"/>
       <c r="F9" s="65"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="96" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-    </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="139" t="s">
+      <c r="B11" s="97"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+    </row>
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="143" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="140"/>
-      <c r="C12" s="140"/>
-      <c r="D12" s="140"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="140"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="144"/>
+      <c r="F12" s="144"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3907,21 +3899,21 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27.109375" customWidth="1"/>
+    <col min="10" max="10" width="27.5546875" customWidth="1"/>
+    <col min="11" max="11" width="26.5546875" customWidth="1"/>
+    <col min="12" max="12" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -3935,97 +3927,97 @@
       </c>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="141" t="s">
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="146" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
-      <c r="J2" s="141"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
-      <c r="E3" s="117" t="s">
+      <c r="E3" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="117"/>
-      <c r="G3" s="118" t="s">
+      <c r="F3" s="94"/>
+      <c r="G3" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="142" t="s">
+    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="92" t="s">
+      <c r="C5" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="98"/>
-      <c r="F5" s="92" t="s">
+      <c r="E5" s="104"/>
+      <c r="F5" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="92" t="s">
+      <c r="G5" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="92" t="s">
+      <c r="I5" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="92" t="s">
+      <c r="J5" s="107" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="142"/>
+    <row r="6" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="147"/>
       <c r="B6" s="99"/>
-      <c r="C6" s="93"/>
+      <c r="C6" s="115"/>
       <c r="D6" s="99"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="99"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-    </row>
-    <row r="7" spans="1:12" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="142"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="94"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+    </row>
+    <row r="7" spans="1:12" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="147"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="116"/>
       <c r="D7" s="52" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -4059,7 +4051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="65">
         <v>1</v>
       </c>
@@ -4073,7 +4065,7 @@
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -4084,37 +4076,37 @@
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="132" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="136" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="132"/>
-      <c r="C11" s="132"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132"/>
-      <c r="H11" s="132"/>
-      <c r="I11" s="132"/>
-      <c r="J11" s="132"/>
-    </row>
-    <row r="13" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="132" t="s">
+      <c r="B11" s="136"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="136"/>
+    </row>
+    <row r="13" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="136" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="132"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132"/>
-      <c r="E13" s="132"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="132"/>
-      <c r="H13" s="132"/>
-      <c r="I13" s="132"/>
-      <c r="J13" s="132"/>
+      <c r="B13" s="136"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="136"/>
+      <c r="G13" s="136"/>
+      <c r="H13" s="136"/>
+      <c r="I13" s="136"/>
+      <c r="J13" s="136"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="1:12" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="53"/>
       <c r="C14" s="53"/>
@@ -4128,37 +4120,37 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="132" t="s">
+    <row r="15" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="132"/>
-      <c r="C15" s="132"/>
-      <c r="D15" s="132"/>
-      <c r="E15" s="132"/>
-      <c r="F15" s="132"/>
-      <c r="G15" s="132"/>
-      <c r="H15" s="132"/>
-      <c r="I15" s="132"/>
-      <c r="J15" s="132"/>
+      <c r="B15" s="136"/>
+      <c r="C15" s="136"/>
+      <c r="D15" s="136"/>
+      <c r="E15" s="136"/>
+      <c r="F15" s="136"/>
+      <c r="G15" s="136"/>
+      <c r="H15" s="136"/>
+      <c r="I15" s="136"/>
+      <c r="J15" s="136"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="132"/>
-      <c r="B16" s="132"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
-      <c r="I16" s="132"/>
-      <c r="J16" s="132"/>
+    <row r="16" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="136"/>
+      <c r="B16" s="136"/>
+      <c r="C16" s="136"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="136"/>
+      <c r="H16" s="136"/>
+      <c r="I16" s="136"/>
+      <c r="J16" s="136"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
@@ -4172,23 +4164,23 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="143" t="s">
+    <row r="18" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="145" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="143"/>
-      <c r="C18" s="143"/>
-      <c r="D18" s="143"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
+      <c r="B18" s="145"/>
+      <c r="C18" s="145"/>
+      <c r="D18" s="145"/>
+      <c r="E18" s="145"/>
+      <c r="F18" s="145"/>
+      <c r="G18" s="145"/>
+      <c r="H18" s="145"/>
+      <c r="I18" s="145"/>
+      <c r="J18" s="145"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -4201,23 +4193,23 @@
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="143" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="143"/>
-      <c r="C20" s="143"/>
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="143"/>
-      <c r="J20" s="143"/>
+      <c r="B20" s="145"/>
+      <c r="C20" s="145"/>
+      <c r="D20" s="145"/>
+      <c r="E20" s="145"/>
+      <c r="F20" s="145"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -4230,7 +4222,7 @@
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -4245,11 +4237,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A15:J16"/>
-    <mergeCell ref="A18:J18"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="J5:J7"/>
@@ -4262,6 +4249,11 @@
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="F5:F7"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A15:J16"/>
+    <mergeCell ref="A18:J18"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -4282,75 +4274,75 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="41" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="41" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="8"/>
       <c r="D1" s="19"/>
       <c r="E1" s="58" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="141" t="s">
+    <row r="2" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B2" s="146" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+    </row>
+    <row r="3" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B3" s="59"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="80" t="s">
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="146"/>
+    </row>
+    <row r="4" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B4" s="111" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="142" t="s">
+    <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="147" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="95" t="s">
+      <c r="E6" s="80" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="142"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="95"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="147"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="80"/>
+    </row>
+    <row r="8" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="49">
         <v>1</v>
       </c>
@@ -4367,7 +4359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="49">
         <v>1</v>
       </c>
@@ -4376,47 +4368,47 @@
       <c r="D9" s="42"/>
       <c r="E9" s="49"/>
     </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="43"/>
       <c r="C10" s="57"/>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="132" t="s">
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="132"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="132"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="132"/>
-      <c r="B13" s="132"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132"/>
-      <c r="E13" s="132"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="136"/>
+      <c r="B13" s="136"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="136"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>92</v>
       </c>
       <c r="B14" s="53"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="16" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="139" t="s">
+    <row r="16" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="143" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="139"/>
-      <c r="C16" s="139"/>
-      <c r="D16" s="139"/>
-      <c r="E16" s="139"/>
-    </row>
-    <row r="23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="25" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="26" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="27" hidden="1" x14ac:dyDescent="0.2"/>
+      <c r="B16" s="143"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="143"/>
+      <c r="E16" s="143"/>
+    </row>
+    <row r="23" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="25" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="26" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="27" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A16:E16"/>
@@ -4447,57 +4439,57 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G1" s="58" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="144" t="s">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+    </row>
+    <row r="3" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="64"/>
       <c r="B3" s="64"/>
       <c r="C3" s="64"/>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="148" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="148"/>
       <c r="G3" s="64"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="D4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="118" t="s">
+      <c r="E4" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="118"/>
+      <c r="F4" s="95"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>5</v>
       </c>
@@ -4520,7 +4512,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>1</v>
       </c>
@@ -4543,7 +4535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="65">
         <v>1</v>
       </c>
@@ -4554,58 +4546,58 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="143" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="139"/>
-      <c r="C10" s="139"/>
-      <c r="D10" s="139"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="139"/>
-      <c r="G10" s="139"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="132" t="s">
+      <c r="B10" s="143"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="143"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="136" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="132"/>
-      <c r="C11" s="132"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132"/>
-    </row>
-    <row r="12" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="139" t="s">
+      <c r="B11" s="136"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+    </row>
+    <row r="12" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="143" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="139"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="139"/>
-    </row>
-    <row r="13" spans="1:8" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="139"/>
-      <c r="B13" s="139"/>
-      <c r="C13" s="139"/>
-      <c r="D13" s="139"/>
-      <c r="E13" s="139"/>
-      <c r="F13" s="139"/>
-      <c r="G13" s="139"/>
-    </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="139" t="s">
+      <c r="B12" s="143"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="143"/>
+      <c r="E12" s="143"/>
+      <c r="F12" s="143"/>
+      <c r="G12" s="143"/>
+    </row>
+    <row r="13" spans="1:8" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="143"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="143"/>
+      <c r="D13" s="143"/>
+      <c r="E13" s="143"/>
+      <c r="F13" s="143"/>
+      <c r="G13" s="143"/>
+    </row>
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="143" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="139"/>
-      <c r="C15" s="139"/>
-      <c r="D15" s="139"/>
-      <c r="E15" s="139"/>
-      <c r="F15" s="139"/>
-      <c r="G15" s="139"/>
+      <c r="B15" s="143"/>
+      <c r="C15" s="143"/>
+      <c r="D15" s="143"/>
+      <c r="E15" s="143"/>
+      <c r="F15" s="143"/>
+      <c r="G15" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>